<commit_message>
formatting for final; updating assessment matrix
</commit_message>
<xml_diff>
--- a/Checklists/NRT COMP MATRIX.xlsx
+++ b/Checklists/NRT COMP MATRIX.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\Apps\2016\NRT-OMeara\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bomeara/Documents/MyDocuments/GitClones/EEB_NRT/Checklists/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16425" windowHeight="12240"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28420" windowHeight="17220"/>
   </bookViews>
   <sheets>
     <sheet name="Comp. Matrix" sheetId="1" r:id="rId1"/>
@@ -18,9 +18,15 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Comp. Matrix'!$A$1:$I$30</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Comp. Matrix'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>RFP Requirement</t>
   </si>
@@ -1306,12 +1312,15 @@
       <t xml:space="preserve"> with nonacademic partners </t>
     </r>
   </si>
+  <si>
+    <t>Done</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1380,6 +1389,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1437,16 +1462,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1477,8 +1502,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1689,7 +1734,27 @@
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="21">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1751,9 +1816,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1786,9 +1851,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1968,28 +2033,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47.5703125" style="19" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5" style="19" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.5" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="29" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="19"/>
+    <col min="8" max="8" width="18.33203125" style="29" customWidth="1"/>
+    <col min="9" max="9" width="9.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.1640625" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2021,7 +2086,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.2">
       <c r="A2" s="36" t="s">
         <v>31</v>
       </c>
@@ -2034,7 +2099,9 @@
       <c r="D2" s="39"/>
       <c r="E2" s="40"/>
       <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="G2" s="42" t="s">
+        <v>45</v>
+      </c>
       <c r="H2" s="38"/>
       <c r="I2" s="43"/>
       <c r="J2" s="32"/>
@@ -2059,7 +2126,7 @@
       <c r="I3" s="36"/>
       <c r="J3" s="32"/>
     </row>
-    <row r="4" spans="1:10" s="15" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" s="15" customFormat="1" ht="154" x14ac:dyDescent="0.2">
       <c r="A4" s="45" t="s">
         <v>32</v>
       </c>
@@ -2073,7 +2140,7 @@
       <c r="I4" s="36"/>
       <c r="J4" s="32"/>
     </row>
-    <row r="5" spans="1:10" s="15" customFormat="1" ht="153" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" s="15" customFormat="1" ht="140" x14ac:dyDescent="0.2">
       <c r="A5" s="37" t="s">
         <v>28</v>
       </c>
@@ -2127,14 +2194,16 @@
       <c r="I7" s="36"/>
       <c r="J7" s="32"/>
     </row>
-    <row r="8" spans="1:10" s="15" customFormat="1" ht="127.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" s="15" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A8" s="38" t="s">
         <v>43</v>
       </c>
       <c r="B8" s="37" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="38"/>
+      <c r="C8" s="38">
+        <v>1</v>
+      </c>
       <c r="D8" s="39"/>
       <c r="E8" s="44"/>
       <c r="F8" s="42"/>
@@ -2143,14 +2212,16 @@
       <c r="I8" s="36"/>
       <c r="J8" s="32"/>
     </row>
-    <row r="9" spans="1:10" s="15" customFormat="1" ht="306" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" s="15" customFormat="1" ht="294" x14ac:dyDescent="0.2">
       <c r="A9" s="43" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="36">
+        <v>3</v>
+      </c>
       <c r="D9" s="36"/>
       <c r="E9" s="36"/>
       <c r="F9" s="36"/>
@@ -2166,7 +2237,9 @@
       <c r="B10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="36">
+        <v>4</v>
+      </c>
       <c r="D10" s="36"/>
       <c r="E10" s="36"/>
       <c r="F10" s="36"/>
@@ -2182,7 +2255,9 @@
       <c r="B11" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="38"/>
+      <c r="C11" s="38">
+        <v>3</v>
+      </c>
       <c r="D11" s="39"/>
       <c r="E11" s="44"/>
       <c r="F11" s="36"/>
@@ -2191,14 +2266,16 @@
       <c r="I11" s="36"/>
       <c r="J11" s="32"/>
     </row>
-    <row r="12" spans="1:10" s="15" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" s="15" customFormat="1" ht="112" x14ac:dyDescent="0.2">
       <c r="A12" s="38" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="38"/>
+      <c r="C12" s="38">
+        <v>1</v>
+      </c>
       <c r="D12" s="39"/>
       <c r="E12" s="44"/>
       <c r="F12" s="36"/>
@@ -2214,7 +2291,9 @@
       <c r="B13" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="38">
+        <v>1</v>
+      </c>
       <c r="D13" s="39"/>
       <c r="E13" s="44"/>
       <c r="F13" s="36"/>
@@ -2230,7 +2309,9 @@
       <c r="B14" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="38"/>
+      <c r="C14" s="38">
+        <v>1</v>
+      </c>
       <c r="D14" s="39"/>
       <c r="E14" s="44"/>
       <c r="F14" s="36"/>
@@ -2239,14 +2320,16 @@
       <c r="I14" s="36"/>
       <c r="J14" s="32"/>
     </row>
-    <row r="15" spans="1:10" s="15" customFormat="1" ht="280.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" s="15" customFormat="1" ht="252" x14ac:dyDescent="0.2">
       <c r="A15" s="38" t="s">
         <v>33</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="38"/>
+      <c r="C15" s="38">
+        <v>2</v>
+      </c>
       <c r="D15" s="39"/>
       <c r="E15" s="44"/>
       <c r="F15" s="36"/>
@@ -2255,14 +2338,16 @@
       <c r="I15" s="36"/>
       <c r="J15" s="32"/>
     </row>
-    <row r="16" spans="1:10" s="15" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="15" customFormat="1" ht="70" x14ac:dyDescent="0.2">
       <c r="A16" s="38" t="s">
         <v>42</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="38"/>
+      <c r="C16" s="38">
+        <v>1</v>
+      </c>
       <c r="D16" s="39"/>
       <c r="E16" s="44"/>
       <c r="F16" s="36"/>
@@ -2278,7 +2363,9 @@
       <c r="B17" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="38">
+        <v>2.5</v>
+      </c>
       <c r="D17" s="39"/>
       <c r="E17" s="44"/>
       <c r="F17" s="36"/>
@@ -2339,7 +2426,7 @@
       <c r="I20" s="36"/>
       <c r="J20" s="32"/>
     </row>
-    <row r="21" spans="1:10" s="15" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" s="15" customFormat="1" ht="196" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>21</v>
       </c>
@@ -2355,7 +2442,7 @@
       <c r="I21" s="36"/>
       <c r="J21" s="32"/>
     </row>
-    <row r="22" spans="1:10" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>22</v>
       </c>
@@ -2369,7 +2456,7 @@
       <c r="I22" s="36"/>
       <c r="J22" s="32"/>
     </row>
-    <row r="23" spans="1:10" s="15" customFormat="1" ht="140.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" s="15" customFormat="1" ht="126" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>23</v>
       </c>
@@ -2383,7 +2470,7 @@
       <c r="I23" s="36"/>
       <c r="J23" s="32"/>
     </row>
-    <row r="24" spans="1:10" s="15" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" s="15" customFormat="1" ht="28" x14ac:dyDescent="0.2">
       <c r="A24" s="37" t="s">
         <v>24</v>
       </c>
@@ -2399,7 +2486,7 @@
       <c r="I24" s="36"/>
       <c r="J24" s="32"/>
     </row>
-    <row r="25" spans="1:10" s="15" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" s="15" customFormat="1" ht="56" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
         <v>38</v>
       </c>
@@ -2431,7 +2518,7 @@
       <c r="I26" s="36"/>
       <c r="J26" s="32"/>
     </row>
-    <row r="27" spans="1:10" s="15" customFormat="1" ht="165.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" s="15" customFormat="1" ht="154" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>40</v>
       </c>
@@ -2449,7 +2536,7 @@
       <c r="I27" s="36"/>
       <c r="J27" s="32"/>
     </row>
-    <row r="28" spans="1:10" s="15" customFormat="1" ht="255" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" s="15" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
         <v>26</v>
       </c>
@@ -2465,7 +2552,7 @@
       <c r="I28" s="36"/>
       <c r="J28" s="32"/>
     </row>
-    <row r="29" spans="1:10" s="15" customFormat="1" ht="408" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:10" s="15" customFormat="1" ht="378" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>30</v>
       </c>
@@ -2811,6 +2898,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006A8D87BEC7CED84B90E4B5699FBE8A3A" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="318e7e7370a7a55c3d89d0a8d97b694b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -2924,22 +3020,21 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A10795F-46BE-4FC1-92F2-92F561C76E56}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DCB00113-9EA6-411F-8BED-F478672EBB27}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2955,7 +3050,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DB821943-8297-4A2E-BC03-C3A4A28387C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2968,12 +3063,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A10795F-46BE-4FC1-92F2-92F561C76E56}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>